<commit_message>
MultiTrack component, StreamResponse blob loading seek issue fix
</commit_message>
<xml_diff>
--- a/Songs.xlsx
+++ b/Songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI\AIDJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A032CA97-5D14-49A2-951F-2F43CB10A874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FC1D6A-9AE4-423B-8DF6-72C764F4C04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{ECF03E3A-1EB1-4F68-8D24-AEDF31EDF4B0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="258">
   <si>
     <t xml:space="preserve"> Chaiyya Chaiyya</t>
   </si>
@@ -798,6 +798,9 @@
   </si>
   <si>
     <t xml:space="preserve"> R Rajkumar</t>
+  </si>
+  <si>
+    <t>Daru badnam</t>
   </si>
 </sst>
 </file>
@@ -905,8 +908,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1EBB9C03-0BF1-4A5F-942D-55D75F8BC231}" name="Table46" displayName="Table46" ref="A1:B201" totalsRowShown="0">
-  <autoFilter ref="A1:B201" xr:uid="{7F2B2566-0E66-44D7-B41A-90FD6DEC1B65}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1EBB9C03-0BF1-4A5F-942D-55D75F8BC231}" name="Table46" displayName="Table46" ref="A1:B202" totalsRowShown="0">
+  <autoFilter ref="A1:B202" xr:uid="{7F2B2566-0E66-44D7-B41A-90FD6DEC1B65}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{164B2ABD-9770-4875-BE07-67842185D1D2}" name="Songs"/>
     <tableColumn id="2" xr3:uid="{C1390F6C-21D8-428F-9319-BD07C2BABC5B}" name="Movie"/>
@@ -2604,10 +2607,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A9C003-6579-4B51-9B9C-E015B43C8EA2}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3822,8 +3825,13 @@
         <v>133</v>
       </c>
     </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A201 A502:A1048576">
+  <conditionalFormatting sqref="A1:A202 A502:A1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>